<commit_message>
update naming in extraction results
</commit_message>
<xml_diff>
--- a/exclusion results based on paper contents.xlsx
+++ b/exclusion results based on paper contents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel Lehner\Desktop\Repos\Paper\MDE4DTs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{B2DD885C-491E-4AA6-BF97-746DFD5F29C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{CFC4FEA4-661F-44DE-B3DE-BEFEDD4963BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="2490" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="296" uniqueCount="90">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="293" uniqueCount="88">
   <si>
     <t>Title</t>
   </si>
@@ -64,15 +64,9 @@
     <t>Measuring the Fidelity of Digital Twin Systems</t>
   </si>
   <si>
-    <t>Challenge/Position Paper</t>
-  </si>
-  <si>
     <t>Digital Twin as Risk-Free Experimentation Aid for Techno-Socio-Economic Systems</t>
   </si>
   <si>
-    <t>No MDE technique used</t>
-  </si>
-  <si>
     <t>Using Trace Alignments for Measuring the Similarity between a Physical and Its Digital Twin</t>
   </si>
   <si>
@@ -196,9 +190,6 @@
     <t>Proof of Concept for a Roundtrip Engineering IS for the New Enterprise in the Industry 4.0 Era</t>
   </si>
   <si>
-    <t>Short Paper (Extended Abstract): &lt;4 Seiten</t>
-  </si>
-  <si>
     <t>Holistic Network Virtualization and Pervasive Network Intelligence for 6G</t>
   </si>
   <si>
@@ -226,9 +217,6 @@
     <t>Semantic digital twins for organizational development</t>
   </si>
   <si>
-    <t>No implementation (e.g. Challenge/Position Paper)</t>
-  </si>
-  <si>
     <t>A pattern catalog for augmenting Digital Twin models with behavior; [Ein Musterkatalog zur Erweiterung von digitalen Zwillingsmodellen um Verhaltenssichten]</t>
   </si>
   <si>
@@ -308,6 +296,12 @@
   </si>
   <si>
     <t>Decision</t>
+  </si>
+  <si>
+    <t>Philosophical, Opinion, or Experience paper</t>
+  </si>
+  <si>
+    <t>No MDE application</t>
   </si>
 </sst>
 </file>
@@ -1173,10 +1167,10 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="67" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomLeft" activeCell="A65" sqref="A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1206,7 +1200,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1235,67 +1229,67 @@
         <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
       <c r="G3" s="4" t="str">
-        <f t="shared" ref="G3:G62" si="0">E3</f>
-        <v>Challenge/Position Paper</v>
+        <f t="shared" ref="G3:G64" si="0">E3</f>
+        <v>Philosophical, Opinion, or Experience paper</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="G4" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>No MDE technique used</v>
+        <v>No MDE application</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G5" s="4" t="str">
         <f>E5</f>
         <v>No Model used</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>6</v>
@@ -1307,25 +1301,25 @@
     </row>
     <row r="7" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="G7" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>No MDE technique used</v>
+        <v>No MDE application</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>6</v>
@@ -1343,28 +1337,28 @@
     </row>
     <row r="9" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="G9" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>No MDE technique used</v>
+        <v>No MDE application</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>6</v>
@@ -1379,25 +1373,25 @@
     </row>
     <row r="11" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="G11" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>No MDE technique used</v>
+        <v>No MDE application</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>6</v>
@@ -1415,28 +1409,28 @@
     </row>
     <row r="13" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="G13" s="4" t="str">
         <f>E13</f>
-        <v>No MDE technique used</v>
+        <v>No MDE application</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>6</v>
@@ -1451,7 +1445,7 @@
     </row>
     <row r="15" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>6</v>
@@ -1469,40 +1463,40 @@
     </row>
     <row r="16" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="G16" s="4" t="str">
         <f>E16</f>
-        <v>No MDE technique used</v>
+        <v>No MDE application</v>
       </c>
     </row>
     <row r="17" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="G17" s="4" t="str">
         <f>D17</f>
-        <v>No MDE technique used</v>
+        <v>No MDE application</v>
       </c>
     </row>
     <row r="18" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>6</v>
@@ -1520,22 +1514,22 @@
     </row>
     <row r="19" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="G19" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>No MDE technique used</v>
+        <v>No MDE application</v>
       </c>
     </row>
     <row r="20" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>6</v>
@@ -1553,67 +1547,67 @@
     </row>
     <row r="21" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="G21" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>No MDE technique used</v>
+        <v>No MDE application</v>
       </c>
     </row>
     <row r="22" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
       <c r="G22" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>Challenge/Position Paper</v>
+        <v>Philosophical, Opinion, or Experience paper</v>
       </c>
     </row>
     <row r="23" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
       <c r="G23" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>Challenge/Position Paper</v>
+        <v>Philosophical, Opinion, or Experience paper</v>
       </c>
     </row>
     <row r="24" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
       <c r="G24" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>Challenge/Position Paper</v>
+        <v>Philosophical, Opinion, or Experience paper</v>
       </c>
     </row>
     <row r="25" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>6</v>
@@ -1631,40 +1625,40 @@
     </row>
     <row r="26" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="G26" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>No MDE technique used</v>
+        <v>No MDE application</v>
       </c>
     </row>
     <row r="27" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="G27" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>No MDE technique used</v>
+        <v>No MDE application</v>
       </c>
     </row>
     <row r="28" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>6</v>
@@ -1682,16 +1676,16 @@
     </row>
     <row r="29" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G29" s="4" t="str">
         <f>D29</f>
@@ -1700,16 +1694,16 @@
     </row>
     <row r="30" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C30" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="G30" s="4" t="str">
         <f>D30</f>
@@ -1718,73 +1712,73 @@
     </row>
     <row r="31" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="G31" s="4" t="str">
         <f>D31</f>
-        <v>No MDE technique used</v>
+        <v>No MDE application</v>
       </c>
     </row>
     <row r="32" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="G32" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>No MDE technique used</v>
+        <v>No MDE application</v>
       </c>
     </row>
     <row r="33" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="G33" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>No MDE technique used</v>
+        <v>No MDE application</v>
       </c>
     </row>
     <row r="34" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="G34" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>No MDE technique used</v>
+        <v>No MDE application</v>
       </c>
     </row>
     <row r="35" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>6</v>
@@ -1802,7 +1796,7 @@
     </row>
     <row r="36" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>6</v>
@@ -1820,7 +1814,7 @@
     </row>
     <row r="37" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>6</v>
@@ -1829,7 +1823,7 @@
         <v>6</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="G37" s="4" t="s">
         <v>6</v>
@@ -1837,7 +1831,7 @@
     </row>
     <row r="38" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>6</v>
@@ -1855,85 +1849,85 @@
     </row>
     <row r="39" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="G39" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>No MDE technique used</v>
+        <v>No MDE application</v>
       </c>
     </row>
     <row r="40" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="G40" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>No MDE technique used</v>
+        <v>No MDE application</v>
       </c>
     </row>
     <row r="41" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="G41" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>No MDE technique used</v>
+        <v>No MDE application</v>
       </c>
     </row>
     <row r="42" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="G42" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>No MDE technique used</v>
+        <v>No MDE application</v>
       </c>
     </row>
     <row r="43" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="G43" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>No MDE technique used</v>
+        <v>No MDE application</v>
       </c>
     </row>
     <row r="44" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>52</v>
+        <v>86</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>6</v>
@@ -1947,49 +1941,49 @@
     </row>
     <row r="45" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
       <c r="G45" s="4"/>
     </row>
     <row r="46" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="G46" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>No MDE technique used</v>
+        <v>No MDE application</v>
       </c>
     </row>
     <row r="47" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="G47" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>No MDE technique used</v>
+        <v>No MDE application</v>
       </c>
     </row>
     <row r="48" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>6</v>
@@ -2007,7 +2001,7 @@
     </row>
     <row r="49" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>6</v>
@@ -2025,7 +2019,7 @@
     </row>
     <row r="50" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>6</v>
@@ -2043,7 +2037,7 @@
     </row>
     <row r="51" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>6</v>
@@ -2061,16 +2055,16 @@
     </row>
     <row r="52" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G52" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2079,121 +2073,123 @@
     </row>
     <row r="53" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
       <c r="G53" s="4" t="str">
         <f>D53</f>
-        <v>Challenge/Position Paper</v>
+        <v>Philosophical, Opinion, or Experience paper</v>
       </c>
     </row>
     <row r="54" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="G54" s="4" t="str">
-        <f t="shared" ref="G54:G55" si="2">D54</f>
-        <v>No MDE technique used</v>
+        <f t="shared" ref="G54:G57" si="2">D54</f>
+        <v>No MDE application</v>
       </c>
     </row>
     <row r="55" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="G55" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>No MDE technique used</v>
+        <v>No MDE application</v>
       </c>
     </row>
     <row r="56" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G56" s="4" t="s">
-        <v>10</v>
+        <v>87</v>
+      </c>
+      <c r="G56" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>No MDE application</v>
       </c>
     </row>
     <row r="57" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
     </row>
     <row r="58" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G58" s="4" t="s">
-        <v>8</v>
+        <v>86</v>
+      </c>
+      <c r="G58" s="4" t="str">
+        <f>E58</f>
+        <v>Philosophical, Opinion, or Experience paper</v>
       </c>
     </row>
     <row r="59" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
       <c r="G59" s="4" t="str">
         <f>E59</f>
-        <v>Challenge/Position Paper</v>
+        <v>Philosophical, Opinion, or Experience paper</v>
       </c>
     </row>
     <row r="60" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>6</v>
@@ -2211,7 +2207,7 @@
     </row>
     <row r="61" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>6</v>
@@ -2229,25 +2225,25 @@
     </row>
     <row r="62" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="G62" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>No MDE technique used</v>
+        <v>No MDE application</v>
       </c>
     </row>
     <row r="63" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>6</v>
@@ -2265,24 +2261,25 @@
     </row>
     <row r="64" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G64" s="4" t="s">
-        <v>10</v>
+      <c r="G64" s="4" t="str">
+        <f>C64</f>
+        <v>No MDE application</v>
       </c>
     </row>
     <row r="65" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>6</v>
@@ -2300,67 +2297,67 @@
     </row>
     <row r="66" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="G66" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>No MDE technique used</v>
+        <v>No MDE application</v>
       </c>
     </row>
     <row r="67" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="G67" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>No MDE technique used</v>
+        <v>No MDE application</v>
       </c>
     </row>
     <row r="68" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="G68" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>No MDE technique used</v>
+        <v>No MDE application</v>
       </c>
     </row>
     <row r="69" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="G69" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>No MDE technique used</v>
+        <v>No MDE application</v>
       </c>
     </row>
     <row r="70" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>6</v>
@@ -2378,7 +2375,7 @@
     </row>
     <row r="71" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>6</v>
@@ -2395,22 +2392,22 @@
     </row>
     <row r="72" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="G72" s="4" t="str">
         <f>D72</f>
-        <v>No MDE technique used</v>
+        <v>No MDE application</v>
       </c>
     </row>
     <row r="73" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>6</v>
@@ -2428,7 +2425,7 @@
     </row>
     <row r="74" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>6</v>
@@ -2446,37 +2443,37 @@
     </row>
     <row r="75" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
       <c r="G75" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>Challenge/Position Paper</v>
+        <v>Philosophical, Opinion, or Experience paper</v>
       </c>
     </row>
     <row r="76" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
       <c r="G76" s="4" t="str">
         <f t="shared" si="4"/>
-        <v>Challenge/Position Paper</v>
+        <v>Philosophical, Opinion, or Experience paper</v>
       </c>
     </row>
     <row r="77" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>6</v>
@@ -2494,7 +2491,7 @@
     </row>
     <row r="78" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>6</v>

</xml_diff>